<commit_message>
version 31-08 implementacion de callback
</commit_message>
<xml_diff>
--- a/Nomenclatura_Drones.xlsx
+++ b/Nomenclatura_Drones.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjcaa\Crazyflie-Matlab_Python\V2 - 29_07\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjcaa\Desktop\Educación\Semestres\5to año - Semestre 10\Diseño e innovación en ingeniería 2\Prototipos\Crazyflie-Matlab-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ED29AB32-BAF9-442F-B455-2846AD619FCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08E098D5-8E7E-45FA-8310-A105F182E5AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E866AF8C-E0E6-4746-B149-421F28C669D7}"/>
   </bookViews>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
-    <t>Nomenclatura para el "drone_number" de la función crazyflie_connect</t>
-  </si>
-  <si>
     <t>drone_number</t>
   </si>
   <si>
@@ -81,6 +78,9 @@
   </si>
   <si>
     <t>radio://0/80/2M/E7E7E7E7D3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nomenclatura para el "drone_number" </t>
   </si>
 </sst>
 </file>
@@ -485,7 +485,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -496,16 +496,16 @@
   <sheetData>
     <row r="1" spans="1:2" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="B1" s="3"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -513,7 +513,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -521,7 +521,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -529,7 +529,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -537,7 +537,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -545,7 +545,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -553,7 +553,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -561,7 +561,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -569,7 +569,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -577,7 +577,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -585,7 +585,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -593,7 +593,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -601,7 +601,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>